<commit_message>
finished renaming files to bids format and putting in new folders, needs to fix NAN in anat name
</commit_message>
<xml_diff>
--- a/BIDS_info.xlsx
+++ b/BIDS_info.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="17780" yWindow="460" windowWidth="21940" windowHeight="28260" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="17780" yWindow="460" windowWidth="21940" windowHeight="28260" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="dataset_description" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="53">
   <si>
     <t>BIDSVersion</t>
   </si>
@@ -171,13 +171,34 @@
   </si>
   <si>
     <t>BIDS_scan_title</t>
+  </si>
+  <si>
+    <t>inplaneT1</t>
+  </si>
+  <si>
+    <t>inplaneT2</t>
+  </si>
+  <si>
+    <t>scan title in NIMS output</t>
+  </si>
+  <si>
+    <t>use REF_BIDS_Name</t>
+  </si>
+  <si>
+    <t>only if functional and &gt;1 scan</t>
+  </si>
+  <si>
+    <t>copy exactly</t>
+  </si>
+  <si>
+    <t>use for ANAT_or_FUNCT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -208,16 +229,50 @@
       <color theme="1"/>
       <name val="Cambria"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Cambria"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -225,91 +280,92 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -726,7 +782,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3">
-    <cfRule type="containsBlanks" dxfId="10" priority="1">
+    <cfRule type="containsBlanks" dxfId="9" priority="1">
       <formula>LEN(TRIM(B3))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -820,27 +876,27 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:C4">
-    <cfRule type="containsBlanks" dxfId="9" priority="5">
+    <cfRule type="containsBlanks" dxfId="8" priority="5">
       <formula>LEN(TRIM(B2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:C11 C5">
-    <cfRule type="containsBlanks" dxfId="8" priority="4">
+    <cfRule type="containsBlanks" dxfId="7" priority="4">
       <formula>LEN(TRIM(B5))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="containsBlanks" dxfId="7" priority="3">
+    <cfRule type="containsBlanks" dxfId="6" priority="3">
       <formula>LEN(TRIM(B5))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D4">
-    <cfRule type="containsBlanks" dxfId="6" priority="2">
+    <cfRule type="containsBlanks" dxfId="5" priority="2">
       <formula>LEN(TRIM(D2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D11">
-    <cfRule type="containsBlanks" dxfId="5" priority="1">
+    <cfRule type="containsBlanks" dxfId="4" priority="1">
       <formula>LEN(TRIM(D5))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -948,7 +1004,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:D1048576">
-    <cfRule type="containsBlanks" dxfId="4" priority="1">
+    <cfRule type="containsBlanks" dxfId="3" priority="1">
       <formula>LEN(TRIM(B1))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -958,60 +1014,71 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="13" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>20</v>
+    <row r="2" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>20</v>
@@ -1019,23 +1086,13 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="4" t="str">
-        <f>tasklist!B2</f>
-        <v>emp</v>
+        <v>33</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -1046,17 +1103,16 @@
         <v>30</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="4">
-        <f>tasklist!B3</f>
-        <v>0</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>21</v>
+      <c r="G5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -1067,17 +1123,16 @@
         <v>30</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D6" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="4">
-        <f>tasklist!B4</f>
-        <v>0</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>21</v>
+      <c r="G6" t="s">
+        <v>47</v>
+      </c>
+      <c r="H6" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -1088,21 +1143,56 @@
         <v>30</v>
       </c>
       <c r="C7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D7" t="s">
         <v>21</v>
       </c>
+      <c r="G7" s="4" t="str">
+        <f>tasklist!B2</f>
+        <v>emp</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="4">
+        <f>tasklist!B3</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>35</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>37</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D9" t="s">
         <v>20</v>
+      </c>
+      <c r="G9" s="4">
+        <f>tasklist!B4</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1146,7 +1236,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B2">
-    <cfRule type="containsBlanks" dxfId="3" priority="1">
+    <cfRule type="containsBlanks" dxfId="2" priority="1">
       <formula>LEN(TRIM(B1))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1187,7 +1277,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B2">
-    <cfRule type="containsBlanks" dxfId="2" priority="1">
+    <cfRule type="containsBlanks" dxfId="1" priority="1">
       <formula>LEN(TRIM(B1))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1199,7 +1289,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
@@ -1228,7 +1318,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B2">
-    <cfRule type="containsBlanks" dxfId="1" priority="1">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(B1))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
added catch for missing folders from subject list
</commit_message>
<xml_diff>
--- a/BIDS_info.xlsx
+++ b/BIDS_info.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="17780" yWindow="460" windowWidth="21940" windowHeight="28260" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="10060" yWindow="460" windowWidth="21940" windowHeight="17460" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="dataset_description" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="56">
   <si>
     <t>BIDSVersion</t>
   </si>
@@ -188,10 +188,19 @@
     <t>only if functional and &gt;1 scan</t>
   </si>
   <si>
-    <t>copy exactly</t>
-  </si>
-  <si>
     <t>use for ANAT_or_FUNCT</t>
+  </si>
+  <si>
+    <t>task-emp_bold</t>
+  </si>
+  <si>
+    <t>task-TASKNAME_bold</t>
+  </si>
+  <si>
+    <t>copy exactly and replace TASKNAME if needed</t>
+  </si>
+  <si>
+    <t>20170608_152333</t>
   </si>
 </sst>
 </file>
@@ -352,15 +361,25 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -795,7 +814,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -906,10 +925,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -962,10 +981,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="B4">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C4" t="s">
         <v>17</v>
@@ -976,10 +995,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C5" t="s">
         <v>17</v>
@@ -990,15 +1009,29 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B6">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C6" t="s">
         <v>17</v>
       </c>
       <c r="D6">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7">
+        <v>104</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7">
         <v>18</v>
       </c>
     </row>
@@ -1016,8 +1049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1027,50 +1060,50 @@
     <col min="3" max="3" width="25.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="7" max="7" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="12" t="s">
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:8" s="13" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="8" t="s">
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="H2" s="12" t="s">
         <v>51</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -1100,7 +1133,7 @@
         <v>34</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1120,7 +1153,7 @@
         <v>34</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -1140,7 +1173,7 @@
         <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="C7">
         <v>3</v>
@@ -1148,9 +1181,8 @@
       <c r="D7" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="4" t="str">
-        <f>tasklist!B2</f>
-        <v>emp</v>
+      <c r="G7" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>21</v>
@@ -1161,7 +1193,7 @@
         <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="C8">
         <v>4</v>

</xml_diff>

<commit_message>
fixed FUNCT -> FUNC
</commit_message>
<xml_diff>
--- a/BIDS_info.xlsx
+++ b/BIDS_info.xlsx
@@ -48,18 +48,12 @@
     <t>F</t>
   </si>
   <si>
-    <t>ANAT_or_FUNCT</t>
-  </si>
-  <si>
     <t>NIMS_scan_title</t>
   </si>
   <si>
     <t>anat</t>
   </si>
   <si>
-    <t>funct</t>
-  </si>
-  <si>
     <t>_3Plane_Loc_fgre</t>
   </si>
   <si>
@@ -117,9 +111,6 @@
     <t>only if functional and &gt;1 scan</t>
   </si>
   <si>
-    <t>use for ANAT_or_FUNCT</t>
-  </si>
-  <si>
     <t>copy exactly and replace TASKNAME if needed</t>
   </si>
   <si>
@@ -130,6 +121,15 @@
   </si>
   <si>
     <t>task-emp</t>
+  </si>
+  <si>
+    <t>ANAT_or_FUNC</t>
+  </si>
+  <si>
+    <t>func</t>
+  </si>
+  <si>
+    <t>use for ANAT_or_FUNC</t>
   </si>
 </sst>
 </file>
@@ -624,7 +624,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B3">
         <v>101</v>
@@ -638,7 +638,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B4">
         <v>102</v>
@@ -652,7 +652,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B5">
         <v>103</v>
@@ -666,7 +666,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B6">
         <v>104</v>
@@ -693,7 +693,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -709,151 +709,151 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F1" s="4"/>
       <c r="G1" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="11" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>26</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
       <c r="G2" s="9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="E5">
         <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C6">
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="E6">
         <v>2</v>
       </c>
       <c r="G6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C7">
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="E7">
         <v>2</v>
       </c>
       <c r="G7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" t="s">
         <v>32</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C8">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="E8">
         <v>2</v>
@@ -863,13 +863,13 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
         <v>13</v>
       </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>

</xml_diff>

<commit_message>
added input parameters and resolved relative filepath
</commit_message>
<xml_diff>
--- a/BIDS_info.xlsx
+++ b/BIDS_info.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="29260" yWindow="460" windowWidth="21940" windowHeight="17460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="21940" yWindow="460" windowWidth="21940" windowHeight="28260" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="participants" sheetId="2" r:id="rId1"/>
@@ -693,7 +693,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
adding task description to xlsx doc
</commit_message>
<xml_diff>
--- a/BIDS_info.xlsx
+++ b/BIDS_info.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="36">
   <si>
     <t>participant_id</t>
   </si>
@@ -130,6 +130,12 @@
   </si>
   <si>
     <t>use for ANAT_or_FUNC</t>
+  </si>
+  <si>
+    <t>full_task_name</t>
+  </si>
+  <si>
+    <t>empathy intervention</t>
   </si>
 </sst>
 </file>
@@ -585,40 +591,42 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="14.1640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>100</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>18</v>
       </c>
     </row>
@@ -626,13 +634,13 @@
       <c r="A3" t="s">
         <v>17</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>101</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>18</v>
       </c>
     </row>
@@ -640,13 +648,13 @@
       <c r="A4" t="s">
         <v>18</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>102</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>18</v>
       </c>
     </row>
@@ -654,13 +662,13 @@
       <c r="A5" t="s">
         <v>19</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>103</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>18</v>
       </c>
     </row>
@@ -668,46 +676,42 @@
       <c r="A6" t="s">
         <v>20</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>104</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>18</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:D1048576">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(B1))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C6" sqref="C6:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5" customWidth="1"/>
+    <col min="4" max="4" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
@@ -715,164 +719,180 @@
         <v>21</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4"/>
+      <c r="H1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="11" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" s="11" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="8"/>
+      <c r="D2" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="8"/>
+      <c r="H2" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="I2" s="10" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5" t="s">
         <v>30</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5">
         <v>1</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>32</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>2</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>22</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6" t="s">
         <v>30</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6">
         <v>2</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>32</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>2</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>23</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
       <c r="B7" t="s">
         <v>30</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7">
         <v>3</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>32</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>2</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
       <c r="B8" t="s">
         <v>30</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8">
         <v>4</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>32</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>2</v>
       </c>
-      <c r="G8" s="2"/>
       <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="2"/>
       <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
now takes argument, prints better output, okay with #folder<#protocol scans
</commit_message>
<xml_diff>
--- a/BIDS_info.xlsx
+++ b/BIDS_info.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="21940" yWindow="460" windowWidth="21940" windowHeight="28260" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="21940" yWindow="460" windowWidth="21940" windowHeight="28260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="participants" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="35">
   <si>
     <t>participant_id</t>
   </si>
@@ -82,9 +82,6 @@
   </si>
   <si>
     <t>20170609_15233</t>
-  </si>
-  <si>
-    <t>20170608_15227</t>
   </si>
   <si>
     <t>20170608_15226</t>
@@ -304,18 +301,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -588,10 +574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -649,7 +635,7 @@
         <v>18</v>
       </c>
       <c r="B4" s="1">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>5</v>
@@ -663,26 +649,12 @@
         <v>19</v>
       </c>
       <c r="B5" s="1">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="1">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="1">
-        <v>104</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="1">
         <v>18</v>
       </c>
     </row>
@@ -695,7 +667,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6:C8"/>
     </sheetView>
   </sheetViews>
@@ -716,19 +688,19 @@
         <v>6</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="5" t="s">
@@ -740,23 +712,23 @@
     </row>
     <row r="2" spans="1:9" s="11" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>24</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>25</v>
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
       <c r="H2" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -786,22 +758,22 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F5">
         <v>2</v>
       </c>
       <c r="H5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I5" t="s">
         <v>7</v>
@@ -812,22 +784,22 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D6">
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F6">
         <v>2</v>
       </c>
       <c r="H6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I6" t="s">
         <v>7</v>
@@ -838,25 +810,25 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D7">
         <v>3</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F7">
         <v>2</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -864,16 +836,16 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D8">
         <v>4</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F8">
         <v>2</v>

</xml_diff>

<commit_message>
cleaned up BIDS info
</commit_message>
<xml_diff>
--- a/BIDS_info.xlsx
+++ b/BIDS_info.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27106"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
+  <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdclark/Desktop/NIMS_to_BIDS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sll-members/fmri/SwiSt/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="21940" yWindow="460" windowWidth="21940" windowHeight="28260" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16000" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="participants" sheetId="2" r:id="rId1"/>
     <sheet name="protocol" sheetId="7" r:id="rId2"/>
+    <sheet name="fieldmap" sheetId="8" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="46">
   <si>
     <t>participant_id</t>
   </si>
@@ -42,9 +43,6 @@
     <t>nims_title</t>
   </si>
   <si>
-    <t>20170609_15238</t>
-  </si>
-  <si>
     <t>F</t>
   </si>
   <si>
@@ -54,51 +52,15 @@
     <t>anat</t>
   </si>
   <si>
-    <t>_3Plane_Loc_fgre</t>
-  </si>
-  <si>
     <t>ASSET_calibration</t>
   </si>
   <si>
-    <t>BOLD_EPI_29mm_2sec</t>
-  </si>
-  <si>
-    <t>T1w_9mm_BRAVO</t>
-  </si>
-  <si>
     <t>run_number</t>
   </si>
   <si>
-    <t>T1w</t>
-  </si>
-  <si>
-    <t>T2w</t>
-  </si>
-  <si>
-    <t>REF_BIDS_NAME</t>
-  </si>
-  <si>
-    <t>REF_BIDS_TYPE</t>
-  </si>
-  <si>
-    <t>20170609_15233</t>
-  </si>
-  <si>
-    <t>20170608_15226</t>
-  </si>
-  <si>
-    <t>20170607_15218</t>
-  </si>
-  <si>
     <t>BIDS_scan_title</t>
   </si>
   <si>
-    <t>inplaneT1</t>
-  </si>
-  <si>
-    <t>inplaneT2</t>
-  </si>
-  <si>
     <t>scan title in NIMS output</t>
   </si>
   <si>
@@ -108,37 +70,112 @@
     <t>only if functional and &gt;1 scan</t>
   </si>
   <si>
-    <t>copy exactly and replace TASKNAME if needed</t>
-  </si>
-  <si>
     <t>repetition_time</t>
   </si>
   <si>
-    <t>task-TASKNAME</t>
-  </si>
-  <si>
-    <t>task-emp</t>
-  </si>
-  <si>
     <t>ANAT_or_FUNC</t>
   </si>
   <si>
     <t>func</t>
   </si>
   <si>
-    <t>use for ANAT_or_FUNC</t>
-  </si>
-  <si>
     <t>full_task_name</t>
   </si>
   <si>
-    <t>empathy intervention</t>
+    <t>M</t>
+  </si>
+  <si>
+    <t>20170709_1311_15436</t>
+  </si>
+  <si>
+    <t>20170710_1918_15441</t>
+  </si>
+  <si>
+    <t>20170712_1910_15454</t>
+  </si>
+  <si>
+    <t>20170713_1949_15463</t>
+  </si>
+  <si>
+    <t>20170714_1812_15473</t>
+  </si>
+  <si>
+    <t>20170716_1621_15490</t>
+  </si>
+  <si>
+    <t>20170807_2040_15690</t>
+  </si>
+  <si>
+    <t>20170808_2005_15700</t>
+  </si>
+  <si>
+    <t>20170814_2010_15770</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3Plane_Loc_fgre </t>
+  </si>
+  <si>
+    <t>BOLD_EPI_29mm_2sec_ToM</t>
+  </si>
+  <si>
+    <t>task-tomloc</t>
+  </si>
+  <si>
+    <t>ToM localizer</t>
+  </si>
+  <si>
+    <t>BOLD_EPI_29mm_2sec_SwiSt</t>
+  </si>
+  <si>
+    <t>task-swist</t>
+  </si>
+  <si>
+    <t>Switch/Stay (main task)</t>
+  </si>
+  <si>
+    <t>sequence</t>
+  </si>
+  <si>
+    <t>intended_for</t>
+  </si>
+  <si>
+    <t>5 6</t>
+  </si>
+  <si>
+    <t>8 9</t>
+  </si>
+  <si>
+    <t>6 7</t>
+  </si>
+  <si>
+    <t>9 10</t>
+  </si>
+  <si>
+    <t>12 13 14</t>
+  </si>
+  <si>
+    <t>11 12</t>
+  </si>
+  <si>
+    <t>14 15 16</t>
+  </si>
+  <si>
+    <t>11 12 13</t>
+  </si>
+  <si>
+    <t>5 6 7 8 10 11 12</t>
+  </si>
+  <si>
+    <t>l</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="000"/>
+  </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -151,11 +188,6 @@
       <sz val="12"/>
       <color rgb="FF222222"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Cambria"/>
     </font>
     <font>
       <b/>
@@ -174,16 +206,27 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="Cambria"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="12"/>
-      <color theme="0"/>
-      <name val="Cambria"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -200,7 +243,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -229,17 +272,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
@@ -259,46 +291,65 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="19">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -354,7 +405,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -389,7 +440,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -574,26 +625,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" style="1"/>
     <col min="4" max="4" width="14.1640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -603,59 +654,129 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1">
-        <v>100</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="A2" s="8">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="8">
         <v>5</v>
       </c>
-      <c r="D2" s="1">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="8">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="1">
-        <v>101</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="1">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="1">
-        <v>103</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="1">
-        <v>18</v>
+      <c r="D4">
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="8">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="8">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="8">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="1">
         <v>19</v>
       </c>
-      <c r="B5" s="1">
-        <v>104</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="1">
-        <v>18</v>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="8">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="8">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="8">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="1">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -665,10 +786,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:C8"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -679,192 +800,644 @@
     <col min="4" max="4" width="25.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="4" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
         <v>33</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" s="11" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" t="s">
-        <v>34</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="F5">
         <v>2</v>
       </c>
-      <c r="H5" t="s">
-        <v>21</v>
-      </c>
-      <c r="I5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D6">
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="F6">
         <v>2</v>
       </c>
-      <c r="H6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D7">
         <v>3</v>
       </c>
       <c r="E7" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="F7">
         <v>2</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I7" t="s">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D8">
         <v>4</v>
       </c>
       <c r="E8" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="F8">
         <v>2</v>
       </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
+      <c r="E9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="24.6640625" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="8">
+        <v>4</v>
+      </c>
+      <c r="B2" s="8" t="str">
+        <f>VLOOKUP(A2,participants!$A$2:$D$10,2)</f>
+        <v>20170709_1311_15436</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="8">
+        <v>4</v>
+      </c>
+      <c r="B3" s="8" t="str">
+        <f>VLOOKUP(A3,participants!$A$2:$D$10,2)</f>
+        <v>20170709_1311_15436</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="8">
+        <v>4</v>
+      </c>
+      <c r="B4" s="8" t="str">
+        <f>VLOOKUP(A4,participants!$A$2:$D$10,2)</f>
+        <v>20170709_1311_15436</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4">
         <v>11</v>
       </c>
-      <c r="B9" t="s">
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="8">
+        <v>5</v>
+      </c>
+      <c r="B5" s="8" t="str">
+        <f>VLOOKUP(A5,participants!$A$2:$D$10,2)</f>
+        <v>20170710_1918_15441</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="8">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8" t="str">
+        <f>VLOOKUP(A6,participants!$A$2:$D$10,2)</f>
+        <v>20170710_1918_15441</v>
+      </c>
+      <c r="C6">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="8">
+        <v>5</v>
+      </c>
+      <c r="B7" s="8" t="str">
+        <f>VLOOKUP(A7,participants!$A$2:$D$10,2)</f>
+        <v>20170710_1918_15441</v>
+      </c>
+      <c r="C7">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="8" t="str">
+        <f>VLOOKUP(A8,participants!$A$2:$D$10,2)</f>
+        <v>20170712_1910_15454</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="8">
+        <v>6</v>
+      </c>
+      <c r="B9" s="8" t="str">
+        <f>VLOOKUP(A9,participants!$A$2:$D$10,2)</f>
+        <v>20170712_1910_15454</v>
+      </c>
+      <c r="C9">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="8">
+        <v>6</v>
+      </c>
+      <c r="B10" s="8" t="str">
+        <f>VLOOKUP(A10,participants!$A$2:$D$10,2)</f>
+        <v>20170712_1910_15454</v>
+      </c>
+      <c r="C10">
         <v>13</v>
       </c>
-      <c r="E9" t="s">
+      <c r="D10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" s="8">
         <v>7</v>
       </c>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
+      <c r="B11" s="8" t="str">
+        <f>VLOOKUP(A11,participants!$A$2:$D$10,2)</f>
+        <v>20170713_1949_15463</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" s="8">
+        <v>7</v>
+      </c>
+      <c r="B12" s="8" t="str">
+        <f>VLOOKUP(A12,participants!$A$2:$D$10,2)</f>
+        <v>20170713_1949_15463</v>
+      </c>
+      <c r="C12">
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" s="8">
+        <v>7</v>
+      </c>
+      <c r="B13" s="8" t="str">
+        <f>VLOOKUP(A13,participants!$A$2:$D$10,2)</f>
+        <v>20170713_1949_15463</v>
+      </c>
+      <c r="C13">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" s="8">
+        <v>8</v>
+      </c>
+      <c r="B14" s="8" t="str">
+        <f>VLOOKUP(A14,participants!$A$2:$D$10,2)</f>
+        <v>20170714_1812_15473</v>
+      </c>
+      <c r="C14">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" s="8">
+        <v>8</v>
+      </c>
+      <c r="B15" s="8" t="str">
+        <f>VLOOKUP(A15,participants!$A$2:$D$10,2)</f>
+        <v>20170714_1812_15473</v>
+      </c>
+      <c r="C15">
+        <v>7</v>
+      </c>
+      <c r="D15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" s="8">
+        <v>8</v>
+      </c>
+      <c r="B16" s="8" t="str">
+        <f>VLOOKUP(A16,participants!$A$2:$D$10,2)</f>
+        <v>20170714_1812_15473</v>
+      </c>
+      <c r="C16">
+        <v>10</v>
+      </c>
+      <c r="D16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="8">
+        <v>9</v>
+      </c>
+      <c r="B17" s="8" t="str">
+        <f>VLOOKUP(A17,participants!$A$2:$D$10,2)</f>
+        <v>20170716_1621_15490</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="8">
+        <v>10</v>
+      </c>
+      <c r="B18" s="8" t="str">
+        <f>VLOOKUP(A18,participants!$A$2:$D$10,2)</f>
+        <v>20170807_2040_15690</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="8">
+        <v>10</v>
+      </c>
+      <c r="B19" s="8" t="str">
+        <f>VLOOKUP(A19,participants!$A$2:$D$10,2)</f>
+        <v>20170807_2040_15690</v>
+      </c>
+      <c r="C19">
+        <v>7</v>
+      </c>
+      <c r="D19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="8">
+        <v>10</v>
+      </c>
+      <c r="B20" s="8" t="str">
+        <f>VLOOKUP(A20,participants!$A$2:$D$10,2)</f>
+        <v>20170807_2040_15690</v>
+      </c>
+      <c r="C20">
+        <v>10</v>
+      </c>
+      <c r="D20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="8">
+        <v>11</v>
+      </c>
+      <c r="B21" s="8" t="str">
+        <f>VLOOKUP(A21,participants!$A$2:$D$10,2)</f>
+        <v>20170808_2005_15700</v>
+      </c>
+      <c r="C21">
+        <v>4</v>
+      </c>
+      <c r="D21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="8">
+        <v>11</v>
+      </c>
+      <c r="B22" s="8" t="str">
+        <f>VLOOKUP(A22,participants!$A$2:$D$10,2)</f>
+        <v>20170808_2005_15700</v>
+      </c>
+      <c r="C22">
+        <v>7</v>
+      </c>
+      <c r="D22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="8">
+        <v>11</v>
+      </c>
+      <c r="B23" s="8" t="str">
+        <f>VLOOKUP(A23,participants!$A$2:$D$10,2)</f>
+        <v>20170808_2005_15700</v>
+      </c>
+      <c r="C23">
+        <v>10</v>
+      </c>
+      <c r="D23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="8">
+        <v>12</v>
+      </c>
+      <c r="B24" s="8" t="str">
+        <f>VLOOKUP(A24,participants!$A$2:$D$10,2)</f>
+        <v>20170814_2010_15770</v>
+      </c>
+      <c r="C24">
+        <v>4</v>
+      </c>
+      <c r="D24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="8">
+        <v>12</v>
+      </c>
+      <c r="B25" s="8" t="str">
+        <f>VLOOKUP(A25,participants!$A$2:$D$10,2)</f>
+        <v>20170814_2010_15770</v>
+      </c>
+      <c r="C25">
+        <v>7</v>
+      </c>
+      <c r="D25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="8">
+        <v>12</v>
+      </c>
+      <c r="B26" s="8" t="str">
+        <f>VLOOKUP(A26,participants!$A$2:$D$10,2)</f>
+        <v>20170814_2010_15770</v>
+      </c>
+      <c r="C26">
+        <v>10</v>
+      </c>
+      <c r="D26" t="s">
+        <v>43</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
changed excel for uh2
</commit_message>
<xml_diff>
--- a/BIDS_info.xlsx
+++ b/BIDS_info.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27526"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10116"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sadevparikh/Desktop/NIMS_to_BIDS/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="5160" yWindow="-26680" windowWidth="25600" windowHeight="15520" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="9" r:id="rId1"/>
@@ -12,20 +17,20 @@
     <sheet name="participants" sheetId="2" r:id="rId3"/>
     <sheet name="protocol" sheetId="7" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="171027"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="63">
   <si>
     <t>participant_id</t>
   </si>
@@ -39,18 +44,12 @@
     <t>nims_title</t>
   </si>
   <si>
-    <t>F</t>
-  </si>
-  <si>
     <t>NIMS_scan_title</t>
   </si>
   <si>
     <t>anat</t>
   </si>
   <si>
-    <t>ASSET_calibration</t>
-  </si>
-  <si>
     <t>run_number</t>
   </si>
   <si>
@@ -69,58 +68,16 @@
     <t>M</t>
   </si>
   <si>
-    <t xml:space="preserve">3Plane_Loc_fgre </t>
-  </si>
-  <si>
-    <t>BOLD_EPI_29mm_2sec_ToM</t>
-  </si>
-  <si>
-    <t>task-tomloc</t>
-  </si>
-  <si>
-    <t>ToM localizer</t>
-  </si>
-  <si>
-    <t>BOLD_EPI_29mm_2sec_SwiSt</t>
-  </si>
-  <si>
-    <t>task-swist</t>
-  </si>
-  <si>
-    <t>5 6</t>
-  </si>
-  <si>
-    <t>8 9</t>
-  </si>
-  <si>
-    <t>11 12 13</t>
-  </si>
-  <si>
-    <t>T1w_9mm_sag</t>
-  </si>
-  <si>
-    <t>T1w</t>
-  </si>
-  <si>
     <t>anat = anatomical, func = functional, fmap = fieldmap</t>
   </si>
   <si>
     <t>nims_title ('default' for default applied across all subjects, specific session IDs for overrides)</t>
   </si>
   <si>
-    <t>default</t>
-  </si>
-  <si>
     <t>sequence_no</t>
   </si>
   <si>
     <t>sequence # in protocol</t>
-  </si>
-  <si>
-    <t>HOShim</t>
-  </si>
-  <si>
-    <t>spiral_fieldmap</t>
   </si>
   <si>
     <t>fmap</t>
@@ -198,6 +155,7 @@
         <sz val="12"/>
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>Required. Dataset name.</t>
@@ -210,15 +168,9 @@
     <t>Optional. Separate each author's name with a comma (NO spaces)</t>
   </si>
   <si>
-    <t>First Author,Second Author</t>
-  </si>
-  <si>
     <t>Research Assistant</t>
   </si>
   <si>
-    <t>My Dataset</t>
-  </si>
-  <si>
     <t>TE (in secs)</t>
   </si>
   <si>
@@ -228,44 +180,65 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>20170709_0900_55555</t>
-  </si>
-  <si>
-    <t>20170710_0900_5556</t>
-  </si>
-  <si>
-    <t>20170711_0900_55557</t>
-  </si>
-  <si>
-    <t>20170712_0900_55558</t>
-  </si>
-  <si>
-    <t>20170713_0900_55559</t>
-  </si>
-  <si>
-    <t>20170714_0900_55560</t>
-  </si>
-  <si>
-    <t>20170715_0900_55561</t>
-  </si>
-  <si>
-    <t>20170716_0900_55562</t>
-  </si>
-  <si>
-    <t>20170717_0900_55563</t>
-  </si>
-  <si>
-    <t>Switch or Stay? (main task)</t>
+    <t>20170223_1106_14450</t>
+  </si>
+  <si>
+    <t>3Plane_Loc_SSFSE</t>
+  </si>
+  <si>
+    <t>HO_Shim</t>
+  </si>
+  <si>
+    <t>task_rest_run_1_sbref</t>
+  </si>
+  <si>
+    <t>task_rest_run_1_ssg</t>
+  </si>
+  <si>
+    <t>task_twoByTwo-run_1_ssg</t>
+  </si>
+  <si>
+    <t>task_ANT_run_1_ssg</t>
+  </si>
+  <si>
+    <t>task_WATT3_run_1_sbref</t>
+  </si>
+  <si>
+    <t>task_WATT3_run_1_ssg</t>
+  </si>
+  <si>
+    <t>task_CCTHot_run_1_ssg</t>
+  </si>
+  <si>
+    <t>task_stopSignal_run_1_ssg</t>
+  </si>
+  <si>
+    <t>fmap_fieldmap</t>
+  </si>
+  <si>
+    <t>anat_T2w</t>
+  </si>
+  <si>
+    <t>T2w</t>
+  </si>
+  <si>
+    <t>task-uh2</t>
+  </si>
+  <si>
+    <t>uh2</t>
+  </si>
+  <si>
+    <t>Sadev Parikh</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -277,6 +250,7 @@
       <sz val="12"/>
       <color rgb="FF222222"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -330,7 +304,20 @@
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF4C7AFF"/>
+      <name val="Andale Mono"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -560,7 +547,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -590,6 +577,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="147">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -756,6 +745,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1016,60 +1008,60 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D14:D15"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="8" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="D2" s="19"/>
       <c r="E2" s="19"/>
@@ -1077,15 +1069,15 @@
       <c r="G2" s="19"/>
       <c r="H2" s="19"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="D3" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1099,79 +1091,68 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="22.6640625" customWidth="1"/>
     <col min="3" max="3" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="16" t="s">
-        <v>11</v>
-      </c>
       <c r="B2" s="14" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="D2" s="17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" t="s">
-        <v>73</v>
-      </c>
       <c r="C3" s="20">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="D3">
         <v>0.03</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="20">
-        <v>2</v>
-      </c>
-      <c r="D4">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C4" s="20"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1185,22 +1166,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.83203125" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" style="1"/>
     <col min="4" max="4" width="14.1640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1214,142 +1195,65 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="10">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>64</v>
+      <c r="B2" s="21" t="s">
+        <v>46</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="D2">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="10">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="10">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="10">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="10">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="1">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="10">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="1">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="10">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="1">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="10">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>71</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="1">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>72</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="1">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="10"/>
+      <c r="C3" s="7"/>
+      <c r="D3"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="10"/>
+      <c r="C4" s="7"/>
+      <c r="D4"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="10"/>
+      <c r="C5" s="7"/>
+      <c r="D5"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="10"/>
+      <c r="C6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="10"/>
+      <c r="C7" s="7"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="10"/>
+      <c r="C8" s="7"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="10"/>
+      <c r="C9" s="7"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="10"/>
+      <c r="C10" s="7"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="9"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="9"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14"/>
     </row>
   </sheetData>
@@ -1364,14 +1268,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.5" customWidth="1"/>
     <col min="2" max="2" width="12.33203125" customWidth="1"/>
@@ -1384,352 +1288,281 @@
     <col min="9" max="9" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F1" s="3" t="s">
+      <c r="I1" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="6" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" s="6" customFormat="1" ht="60">
-      <c r="A2" s="4" t="s">
+      <c r="D2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="G2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>45</v>
-      </c>
       <c r="I2" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" t="s">
-        <v>27</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="22" t="s">
+        <v>46</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="H3" t="str">
         <f>IF(G3="fmap", "Hz", "")</f>
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:9">
-      <c r="A4" t="s">
-        <v>27</v>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="22" t="s">
+        <v>46</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="H4" t="str">
         <f t="shared" ref="H4:H30" si="0">IF(G4="fmap", "Hz", "")</f>
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:9">
-      <c r="A5" t="s">
-        <v>27</v>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="22" t="s">
+        <v>46</v>
       </c>
       <c r="B5">
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="H5" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:9">
-      <c r="A6" t="s">
-        <v>27</v>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="22" t="s">
+        <v>46</v>
       </c>
       <c r="B6">
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="G6" t="s">
-        <v>32</v>
-      </c>
-      <c r="H6" t="str">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" t="s">
+        <v>60</v>
+      </c>
+      <c r="G7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" t="s">
+        <v>60</v>
+      </c>
+      <c r="G9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" t="s">
+        <v>60</v>
+      </c>
+      <c r="G10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" t="s">
+        <v>60</v>
+      </c>
+      <c r="G11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" t="s">
+        <v>60</v>
+      </c>
+      <c r="G12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" t="s">
+        <v>60</v>
+      </c>
+      <c r="G13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" t="str">
         <f t="shared" si="0"/>
         <v>Hz</v>
       </c>
-      <c r="I6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8">
-        <v>6</v>
-      </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8">
-        <v>2</v>
-      </c>
-      <c r="G8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9">
-        <v>7</v>
-      </c>
-      <c r="C9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9">
-        <v>2</v>
-      </c>
-      <c r="G9" t="s">
-        <v>32</v>
-      </c>
-      <c r="H9" t="str">
-        <f t="shared" si="0"/>
-        <v>Hz</v>
-      </c>
-      <c r="I9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10">
-        <v>8</v>
-      </c>
-      <c r="C10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10">
-        <v>3</v>
-      </c>
-      <c r="G10" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11">
-        <v>9</v>
-      </c>
-      <c r="C11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11">
-        <v>4</v>
-      </c>
-      <c r="G11" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12">
-        <v>10</v>
-      </c>
-      <c r="C12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12">
-        <v>3</v>
-      </c>
-      <c r="G12" t="s">
-        <v>32</v>
-      </c>
-      <c r="H12" t="str">
-        <f t="shared" si="0"/>
-        <v>Hz</v>
-      </c>
-      <c r="I12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13">
-        <v>11</v>
-      </c>
-      <c r="C13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13">
-        <v>5</v>
-      </c>
-      <c r="G13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H13" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14">
-        <v>12</v>
-      </c>
-      <c r="C14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" t="s">
-        <v>16</v>
-      </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-      <c r="G14" t="s">
-        <v>12</v>
-      </c>
-      <c r="H14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" t="s">
-        <v>27</v>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="22" t="s">
+        <v>46</v>
       </c>
       <c r="B15">
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
+        <v>58</v>
       </c>
       <c r="D15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15">
-        <v>2</v>
-      </c>
-      <c r="G15" t="s">
-        <v>12</v>
+        <v>59</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="0"/>
@@ -1737,40 +1570,24 @@
       </c>
       <c r="I15" s="12"/>
     </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" s="12">
-        <v>14</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>24</v>
-      </c>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="22"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
-      <c r="G16" s="12" t="s">
-        <v>6</v>
-      </c>
+      <c r="G16" s="12"/>
       <c r="H16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="I16" s="12"/>
     </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="B17" s="12">
-        <v>1</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>14</v>
-      </c>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="12"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
       <c r="D17" s="12"/>
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
@@ -1781,16 +1598,10 @@
       </c>
       <c r="I17" s="12"/>
     </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="B18" s="12">
-        <v>2</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>7</v>
-      </c>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
       <c r="D18" s="12"/>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
@@ -1801,16 +1612,10 @@
       </c>
       <c r="I18" s="12"/>
     </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="B19" s="12">
-        <v>3</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>30</v>
-      </c>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
       <c r="D19" s="15"/>
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
@@ -1821,294 +1626,114 @@
       </c>
       <c r="I19" s="12"/>
     </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="B20" s="12">
-        <v>4</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>33</v>
-      </c>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
       <c r="E20" s="12"/>
-      <c r="F20" s="12">
-        <v>1</v>
-      </c>
-      <c r="G20" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="H20" t="str">
-        <f t="shared" si="0"/>
-        <v>Hz</v>
-      </c>
-      <c r="I20" s="12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="B21" s="12">
-        <v>5</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>19</v>
-      </c>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="I20" s="12"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="12"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
       <c r="E21" s="12"/>
-      <c r="F21" s="12">
-        <v>1</v>
-      </c>
-      <c r="G21" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H21" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
       <c r="I21" s="12"/>
     </row>
-    <row r="22" spans="1:9">
-      <c r="A22" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="B22" s="12">
-        <v>6</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>19</v>
-      </c>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="12"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
       <c r="E22" s="12"/>
-      <c r="F22" s="12">
-        <v>2</v>
-      </c>
-      <c r="G22" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H22" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
       <c r="I22" s="12"/>
     </row>
-    <row r="23" spans="1:9">
-      <c r="A23" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="B23" s="12">
-        <v>7</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>33</v>
-      </c>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="12"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
       <c r="E23" s="12"/>
-      <c r="F23" s="15">
-        <v>2</v>
-      </c>
-      <c r="G23" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="H23" t="str">
-        <f t="shared" si="0"/>
-        <v>Hz</v>
-      </c>
-      <c r="I23" s="12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="A24" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="B24" s="12">
-        <v>8</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D24" s="12" t="s">
-        <v>19</v>
-      </c>
+      <c r="F23" s="15"/>
+      <c r="G23" s="12"/>
+      <c r="I23" s="12"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="12"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
       <c r="E24" s="12"/>
-      <c r="F24" s="12">
-        <v>3</v>
-      </c>
-      <c r="G24" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H24" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
       <c r="I24" s="12"/>
     </row>
-    <row r="25" spans="1:9">
-      <c r="A25" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="B25" s="12">
-        <v>9</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D25" s="12" t="s">
-        <v>19</v>
-      </c>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="12"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
       <c r="E25" s="12"/>
-      <c r="F25" s="12">
-        <v>4</v>
-      </c>
-      <c r="G25" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H25" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
       <c r="I25" s="12"/>
     </row>
-    <row r="26" spans="1:9">
-      <c r="A26" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="B26" s="12">
-        <v>10</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D26" s="12" t="s">
-        <v>33</v>
-      </c>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="12"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
       <c r="E26" s="12"/>
-      <c r="F26" s="15">
-        <v>3</v>
-      </c>
-      <c r="G26" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="H26" t="str">
-        <f t="shared" si="0"/>
-        <v>Hz</v>
-      </c>
-      <c r="I26" s="12">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="A27" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="B27" s="12">
-        <v>11</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D27" s="12" t="s">
-        <v>19</v>
-      </c>
+      <c r="F26" s="15"/>
+      <c r="G26" s="12"/>
+      <c r="I26" s="12"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="12"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
       <c r="E27" s="12"/>
-      <c r="F27" s="12">
-        <v>5</v>
-      </c>
-      <c r="G27" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H27" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
       <c r="I27" s="12"/>
     </row>
-    <row r="28" spans="1:9">
-      <c r="A28" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="B28" s="12">
-        <v>16</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D28" s="12" t="s">
-        <v>16</v>
-      </c>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="12"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
       <c r="E28" s="12"/>
-      <c r="F28" s="12">
-        <v>1</v>
-      </c>
-      <c r="G28" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H28" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
       <c r="I28" s="12"/>
     </row>
-    <row r="29" spans="1:9">
-      <c r="A29" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="B29" s="12">
-        <v>17</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D29" s="12" t="s">
-        <v>16</v>
-      </c>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="12"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
       <c r="E29" s="12"/>
-      <c r="F29" s="12">
-        <v>2</v>
-      </c>
-      <c r="G29" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H29" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
       <c r="I29" s="12"/>
     </row>
-    <row r="30" spans="1:9">
-      <c r="A30" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="B30" s="12">
-        <v>18</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D30" s="12" t="s">
-        <v>24</v>
-      </c>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="12"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
       <c r="E30" s="12"/>
       <c r="F30" s="12"/>
-      <c r="G30" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="H30" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="G30" s="12"/>
       <c r="I30" s="12"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated XLSX with Marissa's input
</commit_message>
<xml_diff>
--- a/BIDS_info.xlsx
+++ b/BIDS_info.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5160" yWindow="-26680" windowWidth="25600" windowHeight="15520" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7040" yWindow="1060" windowWidth="25600" windowHeight="15520" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="9" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="76">
   <si>
     <t>participant_id</t>
   </si>
@@ -229,6 +229,45 @@
   </si>
   <si>
     <t>Sadev Parikh</t>
+  </si>
+  <si>
+    <t>task-rest</t>
+  </si>
+  <si>
+    <t>rest</t>
+  </si>
+  <si>
+    <t>sbref</t>
+  </si>
+  <si>
+    <t>task-twoByTwo</t>
+  </si>
+  <si>
+    <t>task-ANT</t>
+  </si>
+  <si>
+    <t>task-WATT3</t>
+  </si>
+  <si>
+    <t>task-CCTHot</t>
+  </si>
+  <si>
+    <t>task_stopSignal</t>
+  </si>
+  <si>
+    <t>twoByTwo</t>
+  </si>
+  <si>
+    <t>ANT</t>
+  </si>
+  <si>
+    <t>WATT3</t>
+  </si>
+  <si>
+    <t>CCTHot</t>
+  </si>
+  <si>
+    <t>stopSignal</t>
   </si>
 </sst>
 </file>
@@ -1095,7 +1134,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1148,7 +1187,88 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C4" s="20"/>
+      <c r="A4" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="D4">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="D5">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="D6">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="D7">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="D8">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="D9">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
@@ -1272,7 +1392,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1372,7 +1492,7 @@
         <v>48</v>
       </c>
       <c r="H4" t="str">
-        <f t="shared" ref="H4:H30" si="0">IF(G4="fmap", "Hz", "")</f>
+        <f t="shared" ref="H4:H19" si="0">IF(G4="fmap", "Hz", "")</f>
         <v/>
       </c>
     </row>
@@ -1401,11 +1521,14 @@
       <c r="C6" t="s">
         <v>49</v>
       </c>
-      <c r="D6" t="s">
-        <v>60</v>
+      <c r="D6" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -1418,8 +1541,11 @@
       <c r="C7" t="s">
         <v>50</v>
       </c>
-      <c r="D7" t="s">
-        <v>60</v>
+      <c r="D7" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
       </c>
       <c r="G7" t="s">
         <v>10</v>
@@ -1436,7 +1562,10 @@
         <v>51</v>
       </c>
       <c r="D8" t="s">
-        <v>60</v>
+        <v>66</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
       </c>
       <c r="G8" t="s">
         <v>10</v>
@@ -1453,7 +1582,10 @@
         <v>52</v>
       </c>
       <c r="D9" t="s">
-        <v>60</v>
+        <v>67</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
       </c>
       <c r="G9" t="s">
         <v>10</v>
@@ -1470,10 +1602,13 @@
         <v>53</v>
       </c>
       <c r="D10" t="s">
-        <v>60</v>
+        <v>68</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -1487,7 +1622,10 @@
         <v>54</v>
       </c>
       <c r="D11" t="s">
-        <v>60</v>
+        <v>68</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
       </c>
       <c r="G11" t="s">
         <v>10</v>
@@ -1504,7 +1642,10 @@
         <v>55</v>
       </c>
       <c r="D12" t="s">
-        <v>60</v>
+        <v>69</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
       </c>
       <c r="G12" t="s">
         <v>10</v>
@@ -1521,7 +1662,10 @@
         <v>56</v>
       </c>
       <c r="D13" t="s">
-        <v>60</v>
+        <v>70</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
       </c>
       <c r="G13" t="s">
         <v>10</v>
@@ -1540,6 +1684,9 @@
       <c r="D14" t="s">
         <v>17</v>
       </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
       <c r="G14" t="s">
         <v>16</v>
       </c>
@@ -1560,6 +1707,9 @@
       </c>
       <c r="D15" t="s">
         <v>59</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
       </c>
       <c r="G15" s="12" t="s">
         <v>5</v>

</xml_diff>